<commit_message>
Branches Association Products and categories search tool Icons
</commit_message>
<xml_diff>
--- a/Documents/SalesDB.xlsx
+++ b/Documents/SalesDB.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="264"/>
@@ -11,12 +11,12 @@
     <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
     <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
   <si>
     <t>Comments</t>
   </si>
@@ -251,7 +251,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -259,7 +259,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -513,6 +513,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -522,50 +540,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -627,7 +627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -662,7 +662,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -873,51 +873,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J42"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="5" width="21.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="1" customWidth="1"/>
-    <col min="7" max="10" width="21.25" style="1" customWidth="1"/>
+    <col min="2" max="5" width="21.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="21.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1"/>
-    <col min="12" max="14" width="21.375" style="1" customWidth="1"/>
+    <col min="12" max="14" width="21.42578125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="E2" s="25" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E2" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="26"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F2" s="35"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="28"/>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="22" t="s">
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="24"/>
-      <c r="G5" s="22" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="G5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
-    </row>
-    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="30"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>0</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
@@ -951,7 +951,7 @@
       <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
       <c r="G7" s="6"/>
@@ -965,7 +965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="6"/>
       <c r="C8" s="5" t="s">
         <v>49</v>
@@ -987,7 +987,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>53</v>
@@ -1030,7 +1030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="12"/>
       <c r="C12" s="19"/>
       <c r="D12" s="16" t="s">
@@ -1051,14 +1051,14 @@
       <c r="E12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-    </row>
-    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
+    </row>
+    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>55</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="12"/>
       <c r="C14" s="19"/>
       <c r="D14" s="13" t="s">
@@ -1090,17 +1090,17 @@
       <c r="E14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="24" t="s">
         <v>32</v>
       </c>
       <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="35" t="s">
+      <c r="J14" s="23" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="13" t="s">
         <v>21</v>
@@ -1122,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>56</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>56</v>
       </c>
@@ -1179,22 +1179,22 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="22" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
       <c r="G19" s="6"/>
       <c r="I19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="25" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>0</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>32</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
         <v>70</v>
       </c>
@@ -1248,11 +1248,11 @@
       <c r="D22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="39" t="s">
+      <c r="E22" s="27" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>71</v>
       </c>
@@ -1263,14 +1263,14 @@
       <c r="E23" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
-    </row>
-    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="30"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="20" t="s">
@@ -1297,24 +1297,24 @@
       <c r="C25" s="5"/>
       <c r="D25" s="13"/>
       <c r="E25" s="5"/>
-      <c r="G25" s="36"/>
+      <c r="G25" s="24"/>
       <c r="H25" s="1" t="s">
         <v>65</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="26" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="22" t="s">
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="24"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="30"/>
       <c r="G26" s="6"/>
       <c r="H26" s="5" t="s">
         <v>60</v>
@@ -1322,11 +1322,11 @@
       <c r="I26" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="J26" s="39" t="s">
+      <c r="J26" s="27" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>0</v>
       </c>
@@ -1346,11 +1346,11 @@
       <c r="I27" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J27" s="39" t="s">
+      <c r="J27" s="27" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="5" t="s">
         <v>49</v>
@@ -1372,7 +1372,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="5" t="s">
         <v>43</v>
@@ -1394,7 +1394,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="D30" s="13" t="s">
         <v>46</v>
@@ -1413,7 +1413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6"/>
       <c r="C31" s="5"/>
       <c r="D31" s="13" t="s">
@@ -1423,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>55</v>
       </c>
@@ -1434,15 +1434,17 @@
       <c r="E32" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="24"/>
-    </row>
-    <row r="33" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="C33" s="5"/>
       <c r="D33" s="13" t="s">
         <v>29</v>
@@ -1463,8 +1465,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9" t="s">
         <v>29</v>
@@ -1483,7 +1487,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G35" s="6"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
@@ -1493,21 +1497,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B36" s="22" t="s">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="24"/>
-      <c r="G36" s="29" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="30"/>
+      <c r="G36" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="31"/>
-    </row>
-    <row r="37" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="33"/>
+    </row>
+    <row r="37" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="5" t="s">
         <v>49</v>
@@ -1532,12 +1536,12 @@
       <c r="E38" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="24"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="30"/>
     </row>
     <row r="39" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="6"/>
@@ -1563,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="17" t="s">
         <v>35</v>
       </c>
@@ -1585,7 +1589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="G41" s="6"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5" t="s">
@@ -1595,28 +1599,28 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="G42" s="29" t="s">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G42" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
-      <c r="J42" s="31"/>
+      <c r="H42" s="32"/>
+      <c r="I42" s="32"/>
+      <c r="J42" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="B36:E36"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="G32:J32"/>
     <mergeCell ref="G12:J12"/>
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="G36:J36"/>
     <mergeCell ref="E2:G3"/>
     <mergeCell ref="G23:J23"/>
     <mergeCell ref="B19:E19"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="B36:E36"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="G32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1629,7 +1633,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1641,7 +1645,7 @@
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>